<commit_message>
Fix ltdc and ram
</commit_message>
<xml_diff>
--- a/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
+++ b/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="103">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -131,76 +131,214 @@
     <t xml:space="preserve">Widget Wildcard Characters</t>
   </si>
   <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdana.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small</t>
+  </si>
+  <si>
     <t xml:space="preserve">Typography_00</t>
   </si>
   <si>
-    <t xml:space="preserve">digital-7.ttf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
+    <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swmono.ttf</t>
   </si>
   <si>
     <t xml:space="preserve">SingleUseId1</t>
   </si>
   <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swisop3.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Left</t>
   </si>
   <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typography_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Center</t>
+    <t xml:space="preserve">BATT: 14.2V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS : 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTOWY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">' '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATT:  &lt;value&gt; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.9V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT:  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.0 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.0</t>
   </si>
   <si>
     <t xml:space="preserve">Right</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typography_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPM</t>
+    <t xml:space="preserve">SingleUseId14</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JEbać PIS</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1510,7 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1410,13 +1548,13 @@
     </row>
     <row r="5" spans="2:16">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
       <c r="D5">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1452,13 +1590,13 @@
     </row>
     <row r="6" spans="2:16">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1493,6 +1631,33 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1510,6 +1675,33 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1525,6 +1717,33 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1542,6 +1761,33 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -1557,6 +1803,33 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
@@ -1625,104 +1898,223 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working display with can
* Add makefile for internal and external flash

* Add pins for esp

* Set settings for external flash and ram

* Increse flash clock

* Read data from ecumaster can to struct

* Fix ltdc and ram

* Some amazing features

* Test Setup
</commit_message>
<xml_diff>
--- a/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
+++ b/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="103">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -131,76 +131,214 @@
     <t xml:space="preserve">Widget Wildcard Characters</t>
   </si>
   <si>
+    <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verdana.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Large</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Small</t>
+  </si>
+  <si>
     <t xml:space="preserve">Typography_00</t>
   </si>
   <si>
-    <t xml:space="preserve">digital-7.ttf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
+    <t xml:space="preserve">Typography_01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swmono.ttf</t>
   </si>
   <si>
     <t xml:space="preserve">SingleUseId1</t>
   </si>
   <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LTR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swisop3.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Left</t>
   </si>
   <si>
-    <t xml:space="preserve">LTR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">New Text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typography_01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Center</t>
+    <t xml:space="preserve">BATT: 14.2V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS : 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">123458
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overheated!
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ResourceId1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TESTOWY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-9,A-Z,a-z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">' '</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATT:  &lt;value&gt; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.9V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT: 120
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS : &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLT:  &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.0 V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.0</t>
   </si>
   <si>
     <t xml:space="preserve">Right</t>
   </si>
   <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">120</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Typography_02</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RPM</t>
+    <t xml:space="preserve">SingleUseId14</t>
   </si>
   <si>
     <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SingleUseId6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JEbać PIS</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1510,7 @@
         <v>39</v>
       </c>
       <c r="D4">
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1410,13 +1548,13 @@
     </row>
     <row r="5" spans="2:16">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
       <c r="D5">
-        <v>400</v>
+        <v>40</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1452,13 +1590,13 @@
     </row>
     <row r="6" spans="2:16">
       <c r="B6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
         <v>39</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1493,6 +1631,33 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" t="s">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s">
+        <v>40</v>
+      </c>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1510,6 +1675,33 @@
       </c>
     </row>
     <row r="8" spans="2:16">
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8">
+        <v>300</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="J8" t="s">
+        <v>40</v>
+      </c>
       <c r="L8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1525,6 +1717,33 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="2:16">
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>40</v>
+      </c>
       <c r="L9" s="11" t="s">
         <v>6</v>
       </c>
@@ -1542,6 +1761,33 @@
       </c>
     </row>
     <row r="10" spans="2:16">
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>40</v>
+      </c>
       <c r="L10" s="11" t="s">
         <v>28</v>
       </c>
@@ -1557,6 +1803,33 @@
       <c r="P10" s="14"/>
     </row>
     <row r="11" spans="2:16">
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
@@ -1625,104 +1898,223 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="D4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
       <c r="F4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+      <c r="D15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Set oil, gear unkonwn alert
</commit_message>
<xml_diff>
--- a/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
+++ b/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3623" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4063" uniqueCount="114">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -339,6 +339,40 @@
   </si>
   <si>
     <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VINERITC.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL PRESS: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JetBrainsMono-Regular.ttf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BATT: &lt;value&gt; V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OIL PRESS 
+&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26C</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1755,7 @@
         <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="D9">
         <v>40</v>
@@ -1765,7 +1799,7 @@
         <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="D10">
         <v>60</v>
@@ -1833,8 +1867,64 @@
       <c r="L11" s="15"/>
     </row>
     <row r="12" spans="2:16">
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12">
+        <v>60</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
       <c r="M12" s="16" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1918,7 +2008,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
@@ -1944,7 +2034,7 @@
         <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7">
@@ -1961,7 +2051,7 @@
         <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8">
@@ -1978,7 +2068,7 @@
         <v>48</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9">
@@ -2046,7 +2136,7 @@
         <v>48</v>
       </c>
       <c r="F12" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
@@ -2063,15 +2153,15 @@
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="D14" t="s">
         <v>56</v>
@@ -2080,15 +2170,15 @@
         <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
         <v>56</v>
@@ -2097,26 +2187,10 @@
         <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="B16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" t="s">
         <v>102</v>
       </c>
     </row>
+    <row r="16"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Steering wheel status, calc fuel usage
</commit_message>
<xml_diff>
--- a/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
+++ b/Dashboard/Code/Dashboard/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4381" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5253" uniqueCount="210">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -394,6 +394,273 @@
   </si>
   <si>
     <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Typography_07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARAMETER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">val</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId103</t>
   </si>
 </sst>
 </file>
@@ -1927,7 +2194,7 @@
         <v>39</v>
       </c>
       <c r="D13">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E13">
         <v>4</v>
@@ -1945,6 +2212,35 @@
         <v>40</v>
       </c>
       <c r="J13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" t="s">
+        <v>40</v>
+      </c>
+      <c r="H14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2262,6 +2558,1468 @@
         <v>120</v>
       </c>
     </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>126</v>
+      </c>
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>130</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>131</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="F26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="F27" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>133</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" t="s">
+        <v>56</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="F28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F29" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" t="s">
+        <v>48</v>
+      </c>
+      <c r="F30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>136</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" t="s">
+        <v>48</v>
+      </c>
+      <c r="F31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" t="s">
+        <v>48</v>
+      </c>
+      <c r="F33" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>139</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" t="s">
+        <v>48</v>
+      </c>
+      <c r="F34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>140</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>144</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" t="s">
+        <v>48</v>
+      </c>
+      <c r="F39" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>145</v>
+      </c>
+      <c r="C40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" t="s">
+        <v>56</v>
+      </c>
+      <c r="E40" t="s">
+        <v>48</v>
+      </c>
+      <c r="F40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41" t="s">
+        <v>56</v>
+      </c>
+      <c r="E41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F41" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>147</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>56</v>
+      </c>
+      <c r="E42" t="s">
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>148</v>
+      </c>
+      <c r="C43" t="s">
+        <v>110</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" t="s">
+        <v>48</v>
+      </c>
+      <c r="F43" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" t="s">
+        <v>56</v>
+      </c>
+      <c r="E45" t="s">
+        <v>48</v>
+      </c>
+      <c r="F45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
+        <v>56</v>
+      </c>
+      <c r="E46" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" t="s">
+        <v>48</v>
+      </c>
+      <c r="F47" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" t="s">
+        <v>48</v>
+      </c>
+      <c r="F48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>154</v>
+      </c>
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="E49" t="s">
+        <v>48</v>
+      </c>
+      <c r="F49" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>56</v>
+      </c>
+      <c r="E50" t="s">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>156</v>
+      </c>
+      <c r="C51" t="s">
+        <v>110</v>
+      </c>
+      <c r="D51" t="s">
+        <v>56</v>
+      </c>
+      <c r="E51" t="s">
+        <v>48</v>
+      </c>
+      <c r="F51" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>157</v>
+      </c>
+      <c r="C52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>56</v>
+      </c>
+      <c r="E52" t="s">
+        <v>48</v>
+      </c>
+      <c r="F52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>158</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" t="s">
+        <v>56</v>
+      </c>
+      <c r="E53" t="s">
+        <v>48</v>
+      </c>
+      <c r="F53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>159</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s">
+        <v>56</v>
+      </c>
+      <c r="E54" t="s">
+        <v>48</v>
+      </c>
+      <c r="F54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" t="s">
+        <v>56</v>
+      </c>
+      <c r="E55" t="s">
+        <v>48</v>
+      </c>
+      <c r="F55" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>161</v>
+      </c>
+      <c r="C56" t="s">
+        <v>50</v>
+      </c>
+      <c r="D56" t="s">
+        <v>56</v>
+      </c>
+      <c r="E56" t="s">
+        <v>48</v>
+      </c>
+      <c r="F56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>162</v>
+      </c>
+      <c r="C57" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>56</v>
+      </c>
+      <c r="E57" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" t="s">
+        <v>56</v>
+      </c>
+      <c r="E58" t="s">
+        <v>48</v>
+      </c>
+      <c r="F58" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" t="s">
+        <v>56</v>
+      </c>
+      <c r="E59" t="s">
+        <v>48</v>
+      </c>
+      <c r="F59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>165</v>
+      </c>
+      <c r="C60" t="s">
+        <v>50</v>
+      </c>
+      <c r="D60" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" t="s">
+        <v>48</v>
+      </c>
+      <c r="F60" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>166</v>
+      </c>
+      <c r="C61" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" t="s">
+        <v>56</v>
+      </c>
+      <c r="E61" t="s">
+        <v>48</v>
+      </c>
+      <c r="F61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>167</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" t="s">
+        <v>56</v>
+      </c>
+      <c r="E62" t="s">
+        <v>48</v>
+      </c>
+      <c r="F62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>168</v>
+      </c>
+      <c r="C63" t="s">
+        <v>110</v>
+      </c>
+      <c r="D63" t="s">
+        <v>56</v>
+      </c>
+      <c r="E63" t="s">
+        <v>48</v>
+      </c>
+      <c r="F63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>169</v>
+      </c>
+      <c r="C64" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>56</v>
+      </c>
+      <c r="E64" t="s">
+        <v>48</v>
+      </c>
+      <c r="F64" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>170</v>
+      </c>
+      <c r="C65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" t="s">
+        <v>56</v>
+      </c>
+      <c r="E65" t="s">
+        <v>48</v>
+      </c>
+      <c r="F65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>171</v>
+      </c>
+      <c r="C66" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" t="s">
+        <v>56</v>
+      </c>
+      <c r="E66" t="s">
+        <v>48</v>
+      </c>
+      <c r="F66" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>172</v>
+      </c>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" t="s">
+        <v>56</v>
+      </c>
+      <c r="E67" t="s">
+        <v>48</v>
+      </c>
+      <c r="F67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>173</v>
+      </c>
+      <c r="C68" t="s">
+        <v>50</v>
+      </c>
+      <c r="D68" t="s">
+        <v>56</v>
+      </c>
+      <c r="E68" t="s">
+        <v>48</v>
+      </c>
+      <c r="F68" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>174</v>
+      </c>
+      <c r="C69" t="s">
+        <v>110</v>
+      </c>
+      <c r="D69" t="s">
+        <v>56</v>
+      </c>
+      <c r="E69" t="s">
+        <v>48</v>
+      </c>
+      <c r="F69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>175</v>
+      </c>
+      <c r="C70" t="s">
+        <v>50</v>
+      </c>
+      <c r="D70" t="s">
+        <v>56</v>
+      </c>
+      <c r="E70" t="s">
+        <v>48</v>
+      </c>
+      <c r="F70" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" t="s">
+        <v>110</v>
+      </c>
+      <c r="D71" t="s">
+        <v>56</v>
+      </c>
+      <c r="E71" t="s">
+        <v>48</v>
+      </c>
+      <c r="F71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" t="s">
+        <v>48</v>
+      </c>
+      <c r="F72" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>178</v>
+      </c>
+      <c r="C73" t="s">
+        <v>110</v>
+      </c>
+      <c r="D73" t="s">
+        <v>56</v>
+      </c>
+      <c r="E73" t="s">
+        <v>48</v>
+      </c>
+      <c r="F73" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>179</v>
+      </c>
+      <c r="C74" t="s">
+        <v>50</v>
+      </c>
+      <c r="D74" t="s">
+        <v>56</v>
+      </c>
+      <c r="E74" t="s">
+        <v>48</v>
+      </c>
+      <c r="F74" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>180</v>
+      </c>
+      <c r="C75" t="s">
+        <v>110</v>
+      </c>
+      <c r="D75" t="s">
+        <v>56</v>
+      </c>
+      <c r="E75" t="s">
+        <v>48</v>
+      </c>
+      <c r="F75" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>181</v>
+      </c>
+      <c r="C76" t="s">
+        <v>50</v>
+      </c>
+      <c r="D76" t="s">
+        <v>56</v>
+      </c>
+      <c r="E76" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>182</v>
+      </c>
+      <c r="C77" t="s">
+        <v>110</v>
+      </c>
+      <c r="D77" t="s">
+        <v>56</v>
+      </c>
+      <c r="E77" t="s">
+        <v>48</v>
+      </c>
+      <c r="F77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>183</v>
+      </c>
+      <c r="C78" t="s">
+        <v>50</v>
+      </c>
+      <c r="D78" t="s">
+        <v>56</v>
+      </c>
+      <c r="E78" t="s">
+        <v>48</v>
+      </c>
+      <c r="F78" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>184</v>
+      </c>
+      <c r="C79" t="s">
+        <v>110</v>
+      </c>
+      <c r="D79" t="s">
+        <v>56</v>
+      </c>
+      <c r="E79" t="s">
+        <v>48</v>
+      </c>
+      <c r="F79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>185</v>
+      </c>
+      <c r="C80" t="s">
+        <v>50</v>
+      </c>
+      <c r="D80" t="s">
+        <v>56</v>
+      </c>
+      <c r="E80" t="s">
+        <v>48</v>
+      </c>
+      <c r="F80" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>186</v>
+      </c>
+      <c r="C81" t="s">
+        <v>110</v>
+      </c>
+      <c r="D81" t="s">
+        <v>56</v>
+      </c>
+      <c r="E81" t="s">
+        <v>48</v>
+      </c>
+      <c r="F81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>187</v>
+      </c>
+      <c r="C82" t="s">
+        <v>50</v>
+      </c>
+      <c r="D82" t="s">
+        <v>56</v>
+      </c>
+      <c r="E82" t="s">
+        <v>48</v>
+      </c>
+      <c r="F82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>188</v>
+      </c>
+      <c r="C83" t="s">
+        <v>110</v>
+      </c>
+      <c r="D83" t="s">
+        <v>56</v>
+      </c>
+      <c r="E83" t="s">
+        <v>48</v>
+      </c>
+      <c r="F83" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>189</v>
+      </c>
+      <c r="C84" t="s">
+        <v>50</v>
+      </c>
+      <c r="D84" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" t="s">
+        <v>48</v>
+      </c>
+      <c r="F84" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>190</v>
+      </c>
+      <c r="C85" t="s">
+        <v>110</v>
+      </c>
+      <c r="D85" t="s">
+        <v>56</v>
+      </c>
+      <c r="E85" t="s">
+        <v>48</v>
+      </c>
+      <c r="F85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>191</v>
+      </c>
+      <c r="C86" t="s">
+        <v>50</v>
+      </c>
+      <c r="D86" t="s">
+        <v>56</v>
+      </c>
+      <c r="E86" t="s">
+        <v>48</v>
+      </c>
+      <c r="F86" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>192</v>
+      </c>
+      <c r="C87" t="s">
+        <v>110</v>
+      </c>
+      <c r="D87" t="s">
+        <v>56</v>
+      </c>
+      <c r="E87" t="s">
+        <v>48</v>
+      </c>
+      <c r="F87" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" t="s">
+        <v>50</v>
+      </c>
+      <c r="D88" t="s">
+        <v>56</v>
+      </c>
+      <c r="E88" t="s">
+        <v>48</v>
+      </c>
+      <c r="F88" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>194</v>
+      </c>
+      <c r="C89" t="s">
+        <v>110</v>
+      </c>
+      <c r="D89" t="s">
+        <v>56</v>
+      </c>
+      <c r="E89" t="s">
+        <v>48</v>
+      </c>
+      <c r="F89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>195</v>
+      </c>
+      <c r="C90" t="s">
+        <v>50</v>
+      </c>
+      <c r="D90" t="s">
+        <v>56</v>
+      </c>
+      <c r="E90" t="s">
+        <v>48</v>
+      </c>
+      <c r="F90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>196</v>
+      </c>
+      <c r="C91" t="s">
+        <v>110</v>
+      </c>
+      <c r="D91" t="s">
+        <v>56</v>
+      </c>
+      <c r="E91" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>197</v>
+      </c>
+      <c r="C92" t="s">
+        <v>50</v>
+      </c>
+      <c r="D92" t="s">
+        <v>56</v>
+      </c>
+      <c r="E92" t="s">
+        <v>48</v>
+      </c>
+      <c r="F92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>198</v>
+      </c>
+      <c r="C93" t="s">
+        <v>110</v>
+      </c>
+      <c r="D93" t="s">
+        <v>56</v>
+      </c>
+      <c r="E93" t="s">
+        <v>48</v>
+      </c>
+      <c r="F93" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>199</v>
+      </c>
+      <c r="C94" t="s">
+        <v>50</v>
+      </c>
+      <c r="D94" t="s">
+        <v>56</v>
+      </c>
+      <c r="E94" t="s">
+        <v>48</v>
+      </c>
+      <c r="F94" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>200</v>
+      </c>
+      <c r="C95" t="s">
+        <v>110</v>
+      </c>
+      <c r="D95" t="s">
+        <v>56</v>
+      </c>
+      <c r="E95" t="s">
+        <v>48</v>
+      </c>
+      <c r="F95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>201</v>
+      </c>
+      <c r="C96" t="s">
+        <v>50</v>
+      </c>
+      <c r="D96" t="s">
+        <v>56</v>
+      </c>
+      <c r="E96" t="s">
+        <v>48</v>
+      </c>
+      <c r="F96" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>202</v>
+      </c>
+      <c r="C97" t="s">
+        <v>110</v>
+      </c>
+      <c r="D97" t="s">
+        <v>56</v>
+      </c>
+      <c r="E97" t="s">
+        <v>48</v>
+      </c>
+      <c r="F97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>203</v>
+      </c>
+      <c r="C98" t="s">
+        <v>50</v>
+      </c>
+      <c r="D98" t="s">
+        <v>56</v>
+      </c>
+      <c r="E98" t="s">
+        <v>48</v>
+      </c>
+      <c r="F98" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>204</v>
+      </c>
+      <c r="C99" t="s">
+        <v>110</v>
+      </c>
+      <c r="D99" t="s">
+        <v>56</v>
+      </c>
+      <c r="E99" t="s">
+        <v>48</v>
+      </c>
+      <c r="F99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>205</v>
+      </c>
+      <c r="C100" t="s">
+        <v>50</v>
+      </c>
+      <c r="D100" t="s">
+        <v>56</v>
+      </c>
+      <c r="E100" t="s">
+        <v>48</v>
+      </c>
+      <c r="F100" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>206</v>
+      </c>
+      <c r="C101" t="s">
+        <v>110</v>
+      </c>
+      <c r="D101" t="s">
+        <v>56</v>
+      </c>
+      <c r="E101" t="s">
+        <v>48</v>
+      </c>
+      <c r="F101" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>207</v>
+      </c>
+      <c r="C102" t="s">
+        <v>50</v>
+      </c>
+      <c r="D102" t="s">
+        <v>56</v>
+      </c>
+      <c r="E102" t="s">
+        <v>48</v>
+      </c>
+      <c r="F102" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>208</v>
+      </c>
+      <c r="C103" t="s">
+        <v>110</v>
+      </c>
+      <c r="D103" t="s">
+        <v>56</v>
+      </c>
+      <c r="E103" t="s">
+        <v>48</v>
+      </c>
+      <c r="F103" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>209</v>
+      </c>
+      <c r="C104" t="s">
+        <v>50</v>
+      </c>
+      <c r="D104" t="s">
+        <v>56</v>
+      </c>
+      <c r="E104" t="s">
+        <v>48</v>
+      </c>
+      <c r="F104" t="s">
+        <v>125</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>